<commit_message>
Added mayalasian airlines and updated thesis
</commit_message>
<xml_diff>
--- a/ThesisBReport/nomneclature.xlsx
+++ b/ThesisBReport/nomneclature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
   <si>
     <t>ADS-B</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>MEO</t>
-  </si>
-  <si>
-    <t>High Earth Orbit</t>
   </si>
   <si>
     <t>SABIP</t>
@@ -215,6 +212,54 @@
   </si>
   <si>
     <t>MHz, GHz</t>
+  </si>
+  <si>
+    <t>L Band</t>
+  </si>
+  <si>
+    <t>S Band</t>
+  </si>
+  <si>
+    <t>C Band</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t>Medium Earth Orbit</t>
+  </si>
+  <si>
+    <t>IEEE defined electro-magnetic transmission band, between 500 and 1000MHz</t>
+  </si>
+  <si>
+    <t>IEEE defined electro-magnetic transmission band, between 1 and 2GHz</t>
+  </si>
+  <si>
+    <t>IEEE defined electro-magnetic transmission band, between 2 and 4GHz</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Global Positioning Syste</t>
+  </si>
+  <si>
+    <t>GLONASS</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>United States (of America)</t>
+  </si>
+  <si>
+    <t>PSTN</t>
+  </si>
+  <si>
+    <t>Public Switched Telephone Netwok</t>
   </si>
 </sst>
 </file>
@@ -554,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C31"/>
+  <dimension ref="A2:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,262 +620,327 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
         <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C31">
+  <sortState ref="A2:C35">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>